<commit_message>
Update data, fix Reynolds number calculations
</commit_message>
<xml_diff>
--- a/2-semester-molecular-physics/09-mean-free-path/raw/9. Mean free path.xlsx
+++ b/2-semester-molecular-physics/09-mean-free-path/raw/9. Mean free path.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Copy of Sheet1" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="raw" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="results" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>r, [m]</t>
   </si>
@@ -120,10 +120,10 @@
     <t>\Delta lambda</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
     <t>\pm</t>
-  </si>
-  <si>
-    <t>eta \cdot 10^-9</t>
   </si>
   <si>
     <t>\Delta eta \cdot 10^-9</t>
@@ -1002,6 +1002,12 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>997.0</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1019,18 +1025,10 @@
         <v>1.293</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="2">
-        <f>1.6*SQRT(6.1314*$J$1/$J$2)</f>
-        <v>399.0210759</v>
-      </c>
-      <c r="K3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="2">
-        <f>J3*J4</f>
-        <v>0.07584053742</v>
+      <c r="J3" s="1">
+        <v>8.314</v>
       </c>
     </row>
     <row r="4">
@@ -1041,11 +1039,18 @@
         <v>9.81</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J4" s="2">
-        <f>0.005/J1+0.000005/J2</f>
-        <v>0.0001900664952</v>
+        <f>1.6*SQRT($J$3*$J$1/$J$2)</f>
+        <v>464.6447352</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="2">
+        <f>J4*J5</f>
+        <v>0.08831339635</v>
       </c>
     </row>
     <row r="5">
@@ -1056,6 +1061,13 @@
         <f>13.4*10^-2</f>
         <v>0.134</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <f>0.005/J1+0.000005/J2</f>
+        <v>0.0001900664952</v>
+      </c>
     </row>
     <row r="7">
       <c r="E7" s="1"/>
@@ -1091,7 +1103,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>22</v>
@@ -1125,35 +1137,43 @@
         <v>0.102</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G14" si="1">$F$3*$F$4*(D10)</f>
-        <v>1.33185465</v>
+        <f t="shared" ref="G10:G15" si="1">$F$2*$F$4*(D10)</f>
+        <v>1026.95985</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ref="H10:H14" si="2">G10*PI()*$C$1^4*C10/(8*$F$1*$F$5)</f>
-        <v>0.00000006575976802</v>
+        <f t="shared" ref="H10:H15" si="2">G10*PI()*$C$1^4*C10/(8*$F$1*$F$5)</f>
+        <v>0.0000507057144</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" ref="I10:I14" si="3">H10*10^9</f>
-        <v>65.75976802</v>
+        <f t="shared" ref="I10:I15" si="3">H10*10^6</f>
+        <v>50.7057144</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" ref="L10:L14" si="4">$F$1/(PI()*$C$1^2*C10)</f>
+        <f t="shared" ref="L10:L15" si="4">$F$1/(PI()*$C$1^2*C10)</f>
         <v>6.801493295</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" ref="M10:M14" si="5">$C$1*L10*$F$3/H10</f>
-        <v>80240.52785</v>
+        <f t="shared" ref="M10:M15" si="5">$C$1*L10*$F$3/H10</f>
+        <v>104.0631921</v>
       </c>
       <c r="O10" s="2">
-        <f t="shared" ref="O10:O14" si="6">3*H10/($F$3*$J$3)</f>
-        <v>0.0000000003823729548</v>
+        <f t="shared" ref="O10:O15" si="6">3*H10/($F$3*$J$4)</f>
+        <v>0.0000002531970347</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" ref="P10:P14" si="7">O10*10^7</f>
-        <v>0.003823729548</v>
+        <f t="shared" ref="P10:P15" si="7">O10*10^9</f>
+        <v>253.1970347</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" ref="R10:R15" si="8">3*H10/(1.6*$F$3)*SQRT($J$2/($J$3*$J$1))</f>
+        <v>0.0000002531970347</v>
+      </c>
+      <c r="S10" s="2">
+        <f>R10*10^6</f>
+        <v>0.2531970347</v>
       </c>
     </row>
     <row r="11">
@@ -1173,15 +1193,15 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>1.35722331</v>
+        <v>1046.52099</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>0.00000006013927503</v>
+        <v>0.00004637189266</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="3"/>
-        <v>60.13927503</v>
+        <v>46.37189266</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="4"/>
@@ -1189,15 +1209,19 @@
       </c>
       <c r="M11" s="2">
         <f t="shared" si="5"/>
-        <v>97767.03033</v>
+        <v>126.7931497</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="6"/>
-        <v>0.0000000003496915056</v>
+        <v>0.0000002315562625</v>
       </c>
       <c r="P11" s="2">
         <f t="shared" si="7"/>
-        <v>0.003496915056</v>
+        <v>231.5562625</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="8"/>
+        <v>0.0000002315562625</v>
       </c>
     </row>
     <row r="12">
@@ -1217,15 +1241,15 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>0.84985011</v>
+        <v>655.29819</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>0.00000003227768833</v>
+        <v>0.00002488851916</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="3"/>
-        <v>32.27768833</v>
+        <v>24.88851916</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" si="4"/>
@@ -1233,15 +1257,19 @@
       </c>
       <c r="M12" s="2">
         <f t="shared" si="5"/>
-        <v>212517.6368</v>
+        <v>275.6121408</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="6"/>
-        <v>0.0000000001876848935</v>
+        <v>0.0000001242798632</v>
       </c>
       <c r="P12" s="2">
         <f t="shared" si="7"/>
-        <v>0.001876848935</v>
+        <v>124.2798632</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="8"/>
+        <v>0.0000001242798632</v>
       </c>
     </row>
     <row r="13">
@@ -1261,15 +1289,15 @@
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>1.59822558</v>
+        <v>1232.35182</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>0.00000006677145676</v>
+        <v>0.00005148580231</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="3"/>
-        <v>66.77145676</v>
+        <v>51.48580231</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="4"/>
@@ -1277,15 +1305,19 @@
       </c>
       <c r="M13" s="2">
         <f t="shared" si="5"/>
-        <v>93392.90088</v>
+        <v>121.120382</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="6"/>
-        <v>0.0000000003882556156</v>
+        <v>0.0000002570923737</v>
       </c>
       <c r="P13" s="2">
         <f t="shared" si="7"/>
-        <v>0.003882556156</v>
+        <v>257.0923737</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="8"/>
+        <v>0.0000002570923737</v>
       </c>
     </row>
     <row r="14">
@@ -1305,15 +1337,15 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>1.19232702</v>
+        <v>919.37358</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>0.0000000603801533</v>
+        <v>0.00004655762787</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="3"/>
-        <v>60.3801533</v>
+        <v>46.55762787</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="4"/>
@@ -1321,20 +1353,68 @@
       </c>
       <c r="M14" s="2">
         <f t="shared" si="5"/>
-        <v>85204.877</v>
+        <v>110.5014102</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="6"/>
-        <v>0.0000000003510921392</v>
+        <v>0.0000002324837242</v>
       </c>
       <c r="P14" s="2">
         <f t="shared" si="7"/>
-        <v>0.003510921392</v>
+        <v>232.4837242</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="8"/>
+        <v>0.0000002324837242</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D15" s="2">
+        <f>(5.1+3.1)*10^-2</f>
+        <v>0.082</v>
+      </c>
+      <c r="E15" s="2">
+        <f>(2.9+5.1)*10^-2</f>
+        <v>0.08</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>802.00674</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.00005076762614</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="3"/>
+        <v>50.76762614</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="4"/>
+        <v>5.30516477</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="5"/>
+        <v>81.07030289</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="6"/>
+        <v>0.0000002535061886</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="7"/>
+        <v>253.5061886</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="8"/>
+        <v>0.0000002535061886</v>
+      </c>
     </row>
     <row r="17">
       <c r="O17" s="1" t="s">
@@ -1355,34 +1435,34 @@
         <v>37</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" ref="O18:O22" si="8">G19/I10+0.0005/$F$5+$J$4/$J$3</f>
-        <v>0.006826454206</v>
+        <f t="shared" ref="O18:O22" si="9">G19+0.0005/$F$5+$J$5/$J$4</f>
+        <v>0.07390087178</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" ref="P18:P22" si="9">O18*P10</f>
-        <v>0.00002610251465</v>
+        <f t="shared" ref="P18:P22" si="10">O18*P10</f>
+        <v>18.7114816</v>
       </c>
     </row>
     <row r="19">
       <c r="G19" s="2">
-        <f t="shared" ref="G19:G23" si="10">4*(0.00005/$C$1)^3+1/C10+(50*10^-6)/$F$1+0.0005/$F$5 + 0.0005/D10 + 0.0005/$F$3</f>
-        <v>0.2035024528</v>
+        <f t="shared" ref="G19:G23" si="11">4*(0.00005/$C$1)^3+1/C10+(10*10^-6)/$F$1+0.0005/$F$5 + 0.0005/D10 + 0.0005/$F$3</f>
+        <v>0.07016911944</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" ref="H19:H23" si="11">G19*H10</f>
-        <v>0.00000001338227409</v>
+        <f t="shared" ref="H19:H23" si="12">G19*H10</f>
+        <v>0.00000355797533</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" ref="I19:I23" si="12">G19*I10</f>
-        <v>13.38227409</v>
+        <f t="shared" ref="I19:I23" si="13">G19*I10</f>
+        <v>3.55797533</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="8"/>
-        <v>0.007162919309</v>
+        <f t="shared" si="9"/>
+        <v>0.07674226714</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="9"/>
-        <v>0.00002504812038</v>
+        <f t="shared" si="10"/>
+        <v>17.77015256</v>
       </c>
     </row>
     <row r="20">
@@ -1393,82 +1473,82 @@
         <v>34</v>
       </c>
       <c r="G20" s="2">
+        <f t="shared" si="11"/>
+        <v>0.0730105148</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="12"/>
+        <v>0.000003385635755</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="13"/>
+        <v>3.385635755</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="9"/>
+        <v>0.08429396128</v>
+      </c>
+      <c r="P20" s="2">
         <f t="shared" si="10"/>
-        <v>0.2063438481</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="11"/>
-        <v>0.00000001240936943</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="12"/>
-        <v>12.40936943</v>
-      </c>
-      <c r="O20" s="2">
-        <f t="shared" si="8"/>
-        <v>0.01035855013</v>
-      </c>
-      <c r="P20" s="2">
-        <f t="shared" si="9"/>
-        <v>0.00001944143379</v>
+        <v>10.47604197</v>
       </c>
     </row>
     <row r="21">
       <c r="G21" s="2">
+        <f t="shared" si="11"/>
+        <v>0.08056220893</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="12"/>
+        <v>0.00000200507408</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="13"/>
+        <v>2.00507408</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="9"/>
+        <v>0.07776922565</v>
+      </c>
+      <c r="P21" s="2">
         <f t="shared" si="10"/>
-        <v>0.2138955423</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="11"/>
-        <v>0.000000006904053649</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="12"/>
-        <v>6.904053649</v>
-      </c>
-      <c r="O21" s="2">
-        <f t="shared" si="8"/>
-        <v>0.006837500047</v>
-      </c>
-      <c r="P21" s="2">
-        <f t="shared" si="9"/>
-        <v>0.0000265469779</v>
+        <v>19.99387482</v>
       </c>
     </row>
     <row r="22">
       <c r="G22" s="2">
+        <f t="shared" si="11"/>
+        <v>0.07403747331</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="12"/>
+        <v>0.000003811878714</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="13"/>
+        <v>3.811878714</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="9"/>
+        <v>0.07381709031</v>
+      </c>
+      <c r="P22" s="2">
         <f t="shared" si="10"/>
-        <v>0.2073708066</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="11"/>
-        <v>0.00000001384645085</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="12"/>
-        <v>13.84645085</v>
-      </c>
-      <c r="O22" s="2">
-        <f t="shared" si="8"/>
-        <v>0.007100785413</v>
-      </c>
-      <c r="P22" s="2">
-        <f t="shared" si="9"/>
-        <v>0.0000249302994</v>
+        <v>17.16127206</v>
       </c>
     </row>
     <row r="23">
       <c r="G23" s="2">
-        <f t="shared" si="10"/>
-        <v>0.2034186713</v>
+        <f t="shared" si="11"/>
+        <v>0.07008533797</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="11"/>
-        <v>0.00000001228245056</v>
+        <f t="shared" si="12"/>
+        <v>0.000003263007085</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="12"/>
-        <v>12.28245056</v>
+        <f t="shared" si="13"/>
+        <v>3.263007085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>